<commit_message>
check data if import data exist truongTHPT
</commit_message>
<xml_diff>
--- a/XettuyenDGNLTHPT/Uploadtest.xlsx
+++ b/XettuyenDGNLTHPT/Uploadtest.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tuyen\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82702DF2-39D3-4AD1-8FAF-D613364D1670}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EB97FB7-1DFD-416B-ADCE-430335A3B1E2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{C119C5D5-4F9C-4B9A-A7EE-04B094C64F54}"/>
+    <workbookView xWindow="12870" yWindow="3330" windowWidth="15660" windowHeight="12270" xr2:uid="{C119C5D5-4F9C-4B9A-A7EE-04B094C64F54}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="24">
   <si>
     <t>01</t>
   </si>
@@ -49,9 +49,6 @@
     <t>Sở Giáo dục và Đào tạo</t>
   </si>
   <si>
-    <t>800</t>
-  </si>
-  <si>
     <t>Học ở nước ngoài</t>
   </si>
   <si>
@@ -91,19 +88,25 @@
     <t>Trường DTNT</t>
   </si>
   <si>
-    <t>01800</t>
-  </si>
-  <si>
     <t>100</t>
   </si>
   <si>
-    <t>801</t>
-  </si>
-  <si>
     <t>Khu vực 4</t>
   </si>
   <si>
     <t>MãTpTruong</t>
+  </si>
+  <si>
+    <t>1000</t>
+  </si>
+  <si>
+    <t>011000</t>
+  </si>
+  <si>
+    <t>1002</t>
+  </si>
+  <si>
+    <t>011002</t>
   </si>
 </sst>
 </file>
@@ -518,7 +521,7 @@
   <dimension ref="A1:K3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -531,37 +534,37 @@
   <sheetData>
     <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>8</v>
       </c>
-      <c r="B1" t="s">
-        <v>22</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>9</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>10</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>11</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>12</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>13</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>14</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>15</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>16</v>
-      </c>
-      <c r="K1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -569,7 +572,7 @@
         <v>5500</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>0</v>
@@ -584,17 +587,17 @@
         <v>3</v>
       </c>
       <c r="G2" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H2" s="4" t="s">
         <v>4</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>5</v>
       </c>
       <c r="I2" s="4"/>
       <c r="J2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="K2" s="1" t="s">
         <v>6</v>
-      </c>
-      <c r="K2" s="1" t="s">
-        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:11" ht="30" x14ac:dyDescent="0.25">
@@ -602,7 +605,7 @@
         <v>5501</v>
       </c>
       <c r="B3" s="5" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>0</v>
@@ -611,23 +614,23 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>3</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="H3" s="4" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I3" s="4"/>
       <c r="J3" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="K3" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>